<commit_message>
Modelados para la CC 2841209144 Integración activación OSM Micronegocio
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -175,28 +175,28 @@
     <t xml:space="preserve">Mac</t>
   </si>
   <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sin_TotalPlay_TV</t>
   </si>
   <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">PrimeVideo</t>
@@ -1379,7 +1379,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1527,7 +1527,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>1000</v>
+        <v>50</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1553,7 +1553,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="43" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -1579,7 +1579,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="50" t="n">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
@@ -1605,7 +1605,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="43" t="n">
-        <v>200</v>
+        <v>520</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
@@ -1631,7 +1631,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="50" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
@@ -2081,10 +2081,10 @@
         <v>52</v>
       </c>
       <c r="B1" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>53</v>
       </c>
       <c r="D1" s="61" t="s">
         <v>54</v>
@@ -2093,13 +2093,13 @@
         <v>55</v>
       </c>
       <c r="F1" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="60" t="s">
         <v>51</v>
-      </c>
-      <c r="G1" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="60" t="s">
         <v>58</v>
@@ -2125,13 +2125,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="63" t="n">
         <v>20</v>
@@ -2181,13 +2181,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D3" s="66" t="n">
         <v>50</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" s="68" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Agregar framework de automatización de Salesforce ResidencialMicronegocio tv
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -178,25 +178,25 @@
     <t xml:space="preserve">Micronegocio</t>
   </si>
   <si>
+    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
     <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residencial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">PrimeVideo</t>
@@ -629,7 +629,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -850,20 +850,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1137,11 +1125,11 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="82.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="82.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="4.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1224,15 +1212,15 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.14"/>
   </cols>
@@ -1379,22 +1367,22 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="0.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="0.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="17" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="17" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="17" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="17" width="19.99"/>
@@ -1516,7 +1504,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="n">
         <v>1</v>
       </c>
@@ -1542,7 +1530,7 @@
       <c r="O5" s="39"/>
       <c r="P5" s="39"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="n">
         <v>2</v>
       </c>
@@ -1568,7 +1556,7 @@
       <c r="O6" s="47"/>
       <c r="P6" s="47"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="40" t="n">
         <v>3</v>
       </c>
@@ -1594,7 +1582,7 @@
       <c r="O7" s="39"/>
       <c r="P7" s="39"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="n">
         <v>4</v>
       </c>
@@ -1620,7 +1608,7 @@
       <c r="O8" s="47"/>
       <c r="P8" s="47"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="n">
         <v>5</v>
       </c>
@@ -1670,18 +1658,17 @@
       <c r="A11" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
-      <c r="H11" s="57"/>
       <c r="I11" s="50"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
       <c r="N11" s="38"/>
       <c r="O11" s="39"/>
       <c r="P11" s="39"/>
@@ -1690,7 +1677,7 @@
       <c r="A12" s="40" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="42"/>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -1710,18 +1697,17 @@
       <c r="A13" s="40" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
       <c r="G13" s="50"/>
-      <c r="H13" s="57"/>
       <c r="I13" s="50"/>
-      <c r="J13" s="58"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
       <c r="N13" s="38"/>
       <c r="O13" s="39"/>
       <c r="P13" s="39"/>
@@ -1730,7 +1716,7 @@
       <c r="A14" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="59"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="42"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
@@ -1870,18 +1856,17 @@
       <c r="A21" s="40" t="n">
         <v>17</v>
       </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="56"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
-      <c r="H21" s="57"/>
       <c r="I21" s="50"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="58"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
       <c r="N21" s="38"/>
       <c r="O21" s="39"/>
       <c r="P21" s="39"/>
@@ -1890,7 +1875,7 @@
       <c r="A22" s="40" t="n">
         <v>18</v>
       </c>
-      <c r="B22" s="59"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="42"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
@@ -1910,18 +1895,17 @@
       <c r="A23" s="40" t="n">
         <v>19</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
       <c r="G23" s="50"/>
-      <c r="H23" s="57"/>
       <c r="I23" s="50"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="58"/>
-      <c r="M23" s="58"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
       <c r="N23" s="38"/>
       <c r="O23" s="39"/>
       <c r="P23" s="39"/>
@@ -1930,7 +1914,7 @@
       <c r="A24" s="40" t="n">
         <v>20</v>
       </c>
-      <c r="B24" s="59"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="42"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
@@ -2053,7 +2037,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.42"/>
@@ -2068,58 +2052,58 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="60" t="s">
+      <c r="J1" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="60" t="s">
+      <c r="N1" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="62" t="s">
+      <c r="O1" s="59" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2131,12 +2115,12 @@
         <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="63" t="n">
+        <v>51</v>
+      </c>
+      <c r="D2" s="60" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="64" t="n">
+      <c r="E2" s="61" t="n">
         <v>100</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -2169,13 +2153,13 @@
       <c r="O2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="65" t="s">
+      <c r="Q2" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="R2" s="65" t="s">
+      <c r="R2" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="S2" s="65" t="s">
+      <c r="S2" s="62" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2187,12 +2171,12 @@
         <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="66" t="n">
+        <v>57</v>
+      </c>
+      <c r="D3" s="63" t="n">
         <v>50</v>
       </c>
-      <c r="E3" s="67" t="n">
+      <c r="E3" s="64" t="n">
         <v>200</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -2233,10 +2217,10 @@
       <c r="B4" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="69" t="n">
+      <c r="E4" s="66" t="n">
         <v>500</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -2265,10 +2249,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="69" t="n">
+      <c r="E5" s="66" t="n">
         <v>1000</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -2294,10 +2278,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="0" t="n">
         <v>1000</v>
       </c>
@@ -2315,7 +2299,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D7" s="68" t="n">
+      <c r="D7" s="65" t="n">
         <v>1000</v>
       </c>
       <c r="K7" s="0" t="s">

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -175,25 +175,25 @@
     <t xml:space="preserve">Mac</t>
   </si>
   <si>
+    <t xml:space="preserve">Residencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micronegocio</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residencial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
@@ -1125,7 +1125,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.71"/>
@@ -1212,15 +1212,15 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.14"/>
   </cols>
@@ -1367,22 +1367,22 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="0.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="0.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="17" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="17" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="17" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="17" width="19.99"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1538,10 +1538,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="43" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -1564,10 +1564,10 @@
         <v>50</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="50" t="n">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
@@ -1590,10 +1590,10 @@
         <v>50</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="43" t="n">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
@@ -1616,7 +1616,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="50" t="n">
         <v>1000</v>
@@ -1634,7 +1634,7 @@
       <c r="O9" s="39"/>
       <c r="P9" s="39"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
@@ -2037,7 +2037,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.42"/>
@@ -2062,25 +2062,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>55</v>
       </c>
       <c r="F1" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="57" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>51</v>
       </c>
       <c r="H1" s="57" t="s">
         <v>57</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D2" s="60" t="n">
         <v>20</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>55</v>
@@ -2215,7 +2215,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial 200 con promo y crécelo
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -178,16 +178,16 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
   </si>
   <si>
     <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1534,15 +1534,9 @@
       <c r="A6" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="43" t="n">
-        <v>50</v>
-      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -1560,15 +1554,9 @@
       <c r="A7" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="50" t="n">
-        <v>100</v>
-      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -1586,15 +1574,9 @@
       <c r="A8" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="43" t="n">
-        <v>500</v>
-      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -1612,15 +1594,9 @@
       <c r="A9" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="50" t="n">
-        <v>1000</v>
-      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
@@ -2062,22 +2038,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="58" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>51</v>
       </c>
       <c r="E1" s="57" t="s">
         <v>55</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>56</v>
@@ -2112,7 +2088,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>56</v>
@@ -2165,7 +2141,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>55</v>
@@ -2215,7 +2191,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial 50, 100, 500 y 1000
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1534,9 +1534,15 @@
       <c r="A6" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
+      <c r="B6" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="43" t="n">
+        <v>100</v>
+      </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -1554,9 +1560,15 @@
       <c r="A7" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
+      <c r="B7" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="50" t="n">
+        <v>500</v>
+      </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -1574,9 +1586,15 @@
       <c r="A8" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
+      <c r="B8" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="43" t="n">
+        <v>1000</v>
+      </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial 3p 100 cambiar teléfono
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -178,19 +178,19 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
   </si>
   <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1530,7 +1530,7 @@
       <c r="O5" s="39"/>
       <c r="P5" s="39"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="n">
         <v>2</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="43" t="n">
         <v>100</v>
@@ -1560,15 +1560,9 @@
       <c r="A7" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="50" t="n">
-        <v>500</v>
-      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -1586,15 +1580,9 @@
       <c r="A8" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="43" t="n">
-        <v>1000</v>
-      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -2056,22 +2044,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>51</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>56</v>
@@ -2106,7 +2094,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>56</v>
@@ -2159,10 +2147,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>57</v>
@@ -2209,7 +2197,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial 2p BRM
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -178,19 +178,19 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Con_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1538,7 +1538,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="43" t="n">
         <v>100</v>
@@ -1560,9 +1560,15 @@
       <c r="A7" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
+      <c r="B7" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="50" t="n">
+        <v>200</v>
+      </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -1580,9 +1586,15 @@
       <c r="A8" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
+      <c r="B8" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="43" t="n">
+        <v>500</v>
+      </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -1600,9 +1612,15 @@
       <c r="A9" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
+      <c r="B9" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="50" t="n">
+        <v>1000</v>
+      </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
       <c r="G9" s="50"/>
@@ -2044,22 +2062,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="E1" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>55</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>56</v>
@@ -2094,7 +2112,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>56</v>
@@ -2147,10 +2165,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>57</v>
@@ -2197,7 +2215,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial 3p BRM
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -178,19 +178,19 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
   </si>
   <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1541,7 +1541,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="43" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -1567,7 +1567,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="50" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
@@ -1593,7 +1593,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="43" t="n">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
@@ -1619,7 +1619,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="50" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
@@ -1638,9 +1638,15 @@
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
+      <c r="B10" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="53" t="n">
+        <v>1000</v>
+      </c>
       <c r="E10" s="53"/>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -2071,13 +2077,13 @@
         <v>53</v>
       </c>
       <c r="D1" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>51</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>56</v>
@@ -2112,7 +2118,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>56</v>
@@ -2168,7 +2174,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>57</v>
@@ -2215,7 +2221,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial: agregar planes de residencial micronegocio 2p BRM
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -175,18 +175,21 @@
     <t xml:space="preserve">Mac</t>
   </si>
   <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
     <t xml:space="preserve">Con_TotalPlay_TV</t>
   </si>
   <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
   </si>
   <si>
@@ -194,9 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">M_Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
   </si>
   <si>
     <t xml:space="preserve">PrimeVideo</t>
@@ -1122,7 +1122,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="B10:E10 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="B10:E10 F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,7 +1515,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
@@ -1541,7 +1541,7 @@
         <v>51</v>
       </c>
       <c r="D6" s="43" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -1567,7 +1567,7 @@
         <v>51</v>
       </c>
       <c r="D7" s="50" t="n">
-        <v>100</v>
+        <v>220</v>
       </c>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
@@ -1593,7 +1593,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="43" t="n">
-        <v>200</v>
+        <v>520</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
@@ -1619,7 +1619,7 @@
         <v>51</v>
       </c>
       <c r="D9" s="50" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
@@ -1638,15 +1638,9 @@
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="53" t="n">
-        <v>1000</v>
-      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="53"/>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -2040,7 +2034,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="B10:E10 G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2071,25 +2065,25 @@
         <v>52</v>
       </c>
       <c r="B1" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="57" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="57" t="s">
         <v>58</v>
@@ -2115,13 +2109,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="60" t="n">
         <v>20</v>
@@ -2171,13 +2165,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D3" s="63" t="n">
         <v>50</v>
@@ -2221,7 +2215,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial agregar planes de residencial 50mb
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -175,30 +175,36 @@
     <t xml:space="preserve">Mac</t>
   </si>
   <si>
+    <t xml:space="preserve">Residencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netflix Estándar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netflix Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micronegocio</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
+  </si>
+  <si>
     <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
   </si>
   <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residencial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
-  </si>
-  <si>
     <t xml:space="preserve">PrimeVideo</t>
   </si>
   <si>
@@ -211,9 +217,6 @@
     <t xml:space="preserve">WifiExtender</t>
   </si>
   <si>
-    <t xml:space="preserve">Netflix Premium</t>
-  </si>
-  <si>
     <t xml:space="preserve">ZTEF670</t>
   </si>
   <si>
@@ -230,9 +233,6 @@
   </si>
   <si>
     <t xml:space="preserve">Metodo de Pago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Netflix Estándar</t>
   </si>
   <si>
     <t xml:space="preserve">ZTEF660</t>
@@ -629,7 +629,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -778,6 +778,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -806,6 +810,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,6 +839,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1122,7 +1134,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="B10:E10 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,7 +1221,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="B10:E10 F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,7 +1379,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10:E10"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1517,220 +1529,222 @@
       <c r="D5" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="37" t="s">
+        <v>28</v>
+      </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
       <c r="H5" s="21"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="n">
+      <c r="A6" s="41" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="43" t="n">
-        <v>120</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" s="44"/>
+      <c r="F6" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="44"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="n">
+      <c r="A7" s="41" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="50" t="n">
-        <v>220</v>
-      </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="C7" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="52" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="n">
+      <c r="A8" s="41" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="43" t="n">
-        <v>520</v>
-      </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="C8" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="44"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="n">
+      <c r="A9" s="41" t="n">
         <v>5</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="50" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="n">
+      <c r="A11" s="41" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="n">
+      <c r="A12" s="41" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="n">
+      <c r="A13" s="41" t="n">
         <v>9</v>
       </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="n">
+      <c r="A14" s="41" t="n">
         <v>10</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="n">
@@ -1739,196 +1753,196 @@
       <c r="B15" s="34"/>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="n">
+      <c r="A16" s="41" t="n">
         <v>12</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="21"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="47"/>
-      <c r="P16" s="47"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="n">
+      <c r="A17" s="41" t="n">
         <v>13</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
       <c r="H17" s="21"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="n">
+      <c r="A18" s="41" t="n">
         <v>14</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="n">
+      <c r="A19" s="41" t="n">
         <v>15</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="n">
+      <c r="A21" s="41" t="n">
         <v>17</v>
       </c>
       <c r="B21" s="15"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="n">
+      <c r="A22" s="41" t="n">
         <v>18</v>
       </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="47"/>
-      <c r="P22" s="47"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40" t="n">
+      <c r="A23" s="41" t="n">
         <v>19</v>
       </c>
       <c r="B23" s="15"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="40" t="n">
+      <c r="A24" s="41" t="n">
         <v>20</v>
       </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2034,7 +2048,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="B10:E10 G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2061,66 +2075,66 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="57" t="s">
+      <c r="G1" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="H1" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="57" t="s">
+      <c r="K1" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="L1" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="62" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="60" t="n">
+        <v>58</v>
+      </c>
+      <c r="D2" s="63" t="n">
         <v>20</v>
       </c>
-      <c r="E2" s="61" t="n">
+      <c r="E2" s="64" t="n">
         <v>100</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -2136,47 +2150,47 @@
         <v>28</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="62" t="s">
+      <c r="Q2" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="65" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="66" t="n">
         <v>50</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="63" t="n">
-        <v>50</v>
-      </c>
-      <c r="E3" s="64" t="n">
+      <c r="E3" s="67" t="n">
         <v>200</v>
       </c>
       <c r="F3" s="0" t="n">
@@ -2189,7 +2203,7 @@
         <v>120</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>70</v>
@@ -2215,12 +2229,12 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="66" t="n">
+      <c r="E4" s="69" t="n">
         <v>500</v>
       </c>
       <c r="F4" s="0" t="n">
@@ -2249,10 +2263,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="66" t="n">
+      <c r="E5" s="69" t="n">
         <v>1000</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -2278,10 +2292,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="68"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="0" t="n">
         <v>1000</v>
       </c>
@@ -2299,7 +2313,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D7" s="65" t="n">
+      <c r="D7" s="68" t="n">
         <v>1000</v>
       </c>
       <c r="K7" s="0" t="s">

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial agregar planes de residencial cambio…
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -178,61 +178,61 @@
     <t xml:space="preserve">Residencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micronegocio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Con_TotalPlay_TV</t>
   </si>
   <si>
+    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrimeVideo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TipoEquipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TipoSTB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WifiExtender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netflix Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZTEF670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STB 4K - Sagemcom M362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIFI WS 319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si (Manualmente)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecion de paquete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metodo de Pago</t>
+  </si>
+  <si>
     <t xml:space="preserve">Netflix Estándar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Netflix Premium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micronegocio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con_TotalPlay_TV_Y_Video_Soundbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Con_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M_Sin_TotalPlay_TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimeVideo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TipoEquipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TipoSTB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WifiExtender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZTEF670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STB 4K - Sagemcom M362</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIFI WS 319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si (Manualmente)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selecion de paquete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metodo de Pago</t>
   </si>
   <si>
     <t xml:space="preserve">ZTEF660</t>
@@ -1137,7 +1137,7 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.71"/>
@@ -1224,7 +1224,7 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.4"/>
@@ -1379,10 +1379,10 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
@@ -1529,9 +1529,7 @@
       <c r="D5" s="36" t="n">
         <v>50</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>28</v>
-      </c>
+      <c r="E5" s="37"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
       <c r="H5" s="21"/>
@@ -1544,7 +1542,7 @@
       <c r="O5" s="40"/>
       <c r="P5" s="40"/>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="n">
         <v>2</v>
       </c>
@@ -1555,12 +1553,10 @@
         <v>51</v>
       </c>
       <c r="D6" s="44" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E6" s="44"/>
-      <c r="F6" s="45" t="s">
-        <v>52</v>
-      </c>
+      <c r="F6" s="45"/>
       <c r="G6" s="44"/>
       <c r="H6" s="21"/>
       <c r="I6" s="46"/>
@@ -1580,14 +1576,12 @@
         <v>50</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="52" t="n">
-        <v>50</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>28</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E7" s="53"/>
       <c r="F7" s="52"/>
       <c r="G7" s="52"/>
       <c r="H7" s="21"/>
@@ -1608,15 +1602,13 @@
         <v>50</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="44" t="n">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E8" s="44"/>
-      <c r="F8" s="45" t="s">
-        <v>54</v>
-      </c>
+      <c r="F8" s="45"/>
       <c r="G8" s="44"/>
       <c r="H8" s="21"/>
       <c r="I8" s="46"/>
@@ -2051,7 +2043,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.42"/>
@@ -2076,43 +2068,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="60" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="60" t="s">
+      <c r="H1" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="60" t="s">
+      <c r="I1" s="60" t="s">
         <v>58</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="60" t="s">
-        <v>60</v>
       </c>
       <c r="J1" s="60" t="s">
         <v>40</v>
       </c>
       <c r="K1" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="60" t="s">
         <v>61</v>
-      </c>
-      <c r="L1" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="60" t="s">
-        <v>63</v>
       </c>
       <c r="N1" s="60" t="s">
         <v>41</v>
@@ -2126,10 +2118,10 @@
         <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" s="63" t="n">
         <v>20</v>
@@ -2150,28 +2142,28 @@
         <v>28</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="K2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>28</v>
       </c>
       <c r="Q2" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="65" t="s">
         <v>68</v>
-      </c>
-      <c r="R2" s="65" t="s">
-        <v>69</v>
       </c>
       <c r="S2" s="65" t="s">
         <v>17</v>
@@ -2179,13 +2171,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="D3" s="66" t="n">
         <v>50</v>
@@ -2203,7 +2195,7 @@
         <v>120</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>70</v>
@@ -2229,7 +2221,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="68" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
test(web)/qa/salesforce/residencial agregar planes de residencial validación ambientes nube
</commit_message>
<xml_diff>
--- a/inputs/ActivationFluxConfiguration.xlsx
+++ b/inputs/ActivationFluxConfiguration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
   <si>
     <t xml:space="preserve">Proyecto</t>
   </si>
@@ -1134,10 +1134,10 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="B6:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.71"/>
@@ -1221,10 +1221,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="B6:D8 F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.4"/>
@@ -1379,10 +1379,10 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
@@ -1527,7 +1527,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="36" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="36"/>
@@ -1546,15 +1546,9 @@
       <c r="A6" s="41" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="44" t="n">
-        <v>100</v>
-      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="44"/>
       <c r="F6" s="45"/>
       <c r="G6" s="44"/>
@@ -1572,15 +1566,9 @@
       <c r="A7" s="41" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="52" t="n">
-        <v>200</v>
-      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="53"/>
       <c r="F7" s="52"/>
       <c r="G7" s="52"/>
@@ -1598,15 +1586,9 @@
       <c r="A8" s="41" t="n">
         <v>4</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="44" t="n">
-        <v>500</v>
-      </c>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="44"/>
       <c r="F8" s="45"/>
       <c r="G8" s="44"/>
@@ -2040,10 +2022,10 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="B6:D8 G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.42"/>

</xml_diff>